<commit_message>
Sigue sin salirnos MIGUEL 2 VECES
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES BERLANGA-ANDALUZ PRUEBA.xlsx
+++ b/src/main/resources/MEDICIONES BERLANGA-ANDALUZ PRUEBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCB7128-9307-4A7F-9C93-BF0635A47A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A46B238-753F-4C1D-9417-FE8A9651297F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
+    <workbookView xWindow="32025" yWindow="2595" windowWidth="23580" windowHeight="12360" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
   <sheets>
     <sheet name="linea" sheetId="3" r:id="rId1"/>
@@ -765,6 +765,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -809,39 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1163,7 +1163,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,19 +1180,19 @@
   <sheetData>
     <row r="1" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1298,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="31">
-        <v>45060</v>
+        <v>45059</v>
       </c>
       <c r="K7" s="32" t="s">
         <v>35</v>
@@ -1646,13 +1646,13 @@
       <c r="I20" s="21"/>
     </row>
     <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1660,10 +1660,10 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="54"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="5" t="s">
         <v>7</v>
       </c>
@@ -1673,17 +1673,17 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="55">
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="66">
         <f>C20</f>
         <v>4.4219999999999997</v>
       </c>
-      <c r="G25" s="56"/>
+      <c r="G25" s="67"/>
       <c r="H25" s="1">
         <v>4600</v>
       </c>
@@ -1694,17 +1694,17 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="55">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="66">
         <f>D20</f>
         <v>101</v>
       </c>
-      <c r="G26" s="56"/>
+      <c r="G26" s="67"/>
       <c r="H26" s="1">
         <v>1200</v>
       </c>
@@ -1715,17 +1715,17 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="55">
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="66">
         <f>E20</f>
         <v>44.776000000000003</v>
       </c>
-      <c r="G27" s="56"/>
+      <c r="G27" s="67"/>
       <c r="H27" s="1">
         <v>9200</v>
       </c>
@@ -1736,17 +1736,17 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="57">
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="68">
         <f>H20</f>
         <v>1378</v>
       </c>
-      <c r="G28" s="57"/>
+      <c r="G28" s="68"/>
       <c r="H28" s="2">
         <v>2500</v>
       </c>
@@ -1757,15 +1757,15 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
       <c r="I29" s="14"/>
       <c r="J29" s="3">
         <f>SUM(J25:J28)</f>
@@ -1805,17 +1805,17 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="59">
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="44">
         <f>F19</f>
         <v>14</v>
       </c>
-      <c r="G33" s="59"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="1">
         <v>250</v>
       </c>
@@ -1826,17 +1826,17 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66">
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="51">
         <f>G19</f>
         <v>868</v>
       </c>
-      <c r="G34" s="67"/>
+      <c r="G34" s="52"/>
       <c r="H34" s="1">
         <v>24</v>
       </c>
@@ -1847,17 +1847,17 @@
       </c>
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="66">
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="51">
         <f>I19</f>
         <v>33</v>
       </c>
-      <c r="G35" s="68"/>
+      <c r="G35" s="53"/>
       <c r="H35" s="1">
         <v>50</v>
       </c>
@@ -1868,16 +1868,16 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="59">
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="44">
         <v>0</v>
       </c>
-      <c r="G36" s="59"/>
+      <c r="G36" s="44"/>
       <c r="H36" s="1">
         <v>90</v>
       </c>
@@ -1888,16 +1888,16 @@
       </c>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="59">
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="44">
         <v>0</v>
       </c>
-      <c r="G37" s="59"/>
+      <c r="G37" s="44"/>
       <c r="H37" s="1">
         <v>240.45</v>
       </c>
@@ -1909,14 +1909,14 @@
       <c r="L37" s="17"/>
     </row>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="1">
         <v>10</v>
       </c>
@@ -1928,18 +1928,18 @@
       <c r="L38" s="17"/>
     </row>
     <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="69" t="s">
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
       <c r="J39" s="1"/>
       <c r="L39" s="17"/>
     </row>
@@ -1947,10 +1947,10 @@
       <c r="L40" s="17"/>
     </row>
     <row r="41" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G41" s="60" t="s">
+      <c r="G41" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="61"/>
+      <c r="H41" s="46"/>
       <c r="I41" s="16"/>
       <c r="J41" s="3">
         <f>J31+J33+J36+J37+J34+J35+J38+J39</f>
@@ -1966,6 +1966,18 @@
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="27">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B36:E36"/>
@@ -1981,18 +1993,6 @@
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Si quito MIGUEL y pongo otro JUAN, se actualiza bien (no entiendo)
</commit_message>
<xml_diff>
--- a/src/main/resources/MEDICIONES BERLANGA-ANDALUZ PRUEBA.xlsx
+++ b/src/main/resources/MEDICIONES BERLANGA-ANDALUZ PRUEBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A46B238-753F-4C1D-9417-FE8A9651297F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B43CB96-0A92-4E5E-92C8-DF718FC3400F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="2595" windowWidth="23580" windowHeight="12360" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
+    <workbookView xWindow="31755" yWindow="1935" windowWidth="23580" windowHeight="12360" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
   <sheets>
     <sheet name="linea" sheetId="3" r:id="rId1"/>
@@ -765,6 +765,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,51 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1163,7 +1163,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,19 +1180,19 @@
   <sheetData>
     <row r="1" spans="2:12" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="2:12" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1247,7 +1247,7 @@
         <v>45068</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="L5" s="37" t="s">
         <v>38</v>
@@ -1646,13 +1646,13 @@
       <c r="I20" s="21"/>
     </row>
     <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
       <c r="I23" s="13"/>
     </row>
     <row r="24" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1660,10 +1660,10 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="64" t="s">
+      <c r="F24" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="65"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="5" t="s">
         <v>7</v>
       </c>
@@ -1673,17 +1673,17 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="66">
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="55">
         <f>C20</f>
         <v>4.4219999999999997</v>
       </c>
-      <c r="G25" s="67"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="1">
         <v>4600</v>
       </c>
@@ -1694,17 +1694,17 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="66">
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="55">
         <f>D20</f>
         <v>101</v>
       </c>
-      <c r="G26" s="67"/>
+      <c r="G26" s="56"/>
       <c r="H26" s="1">
         <v>1200</v>
       </c>
@@ -1715,17 +1715,17 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="66">
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="55">
         <f>E20</f>
         <v>44.776000000000003</v>
       </c>
-      <c r="G27" s="67"/>
+      <c r="G27" s="56"/>
       <c r="H27" s="1">
         <v>9200</v>
       </c>
@@ -1736,17 +1736,17 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="69" t="s">
+      <c r="B28" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="68">
+      <c r="C28" s="58"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="57">
         <f>H20</f>
         <v>1378</v>
       </c>
-      <c r="G28" s="68"/>
+      <c r="G28" s="57"/>
       <c r="H28" s="2">
         <v>2500</v>
       </c>
@@ -1757,15 +1757,15 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="14"/>
       <c r="J29" s="3">
         <f>SUM(J25:J28)</f>
@@ -1805,17 +1805,17 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="44">
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="59">
         <f>F19</f>
         <v>14</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="59"/>
       <c r="H33" s="1">
         <v>250</v>
       </c>
@@ -1826,17 +1826,17 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="51">
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="66">
         <f>G19</f>
         <v>868</v>
       </c>
-      <c r="G34" s="52"/>
+      <c r="G34" s="67"/>
       <c r="H34" s="1">
         <v>24</v>
       </c>
@@ -1847,17 +1847,17 @@
       </c>
     </row>
     <row r="35" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="51">
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="66">
         <f>I19</f>
         <v>33</v>
       </c>
-      <c r="G35" s="53"/>
+      <c r="G35" s="68"/>
       <c r="H35" s="1">
         <v>50</v>
       </c>
@@ -1868,16 +1868,16 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="44">
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="59">
         <v>0</v>
       </c>
-      <c r="G36" s="44"/>
+      <c r="G36" s="59"/>
       <c r="H36" s="1">
         <v>90</v>
       </c>
@@ -1888,16 +1888,16 @@
       </c>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="44">
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="59">
         <v>0</v>
       </c>
-      <c r="G37" s="44"/>
+      <c r="G37" s="59"/>
       <c r="H37" s="1">
         <v>240.45</v>
       </c>
@@ -1909,14 +1909,14 @@
       <c r="L37" s="17"/>
     </row>
     <row r="38" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
       <c r="H38" s="1">
         <v>10</v>
       </c>
@@ -1928,18 +1928,18 @@
       <c r="L38" s="17"/>
     </row>
     <row r="39" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="54" t="s">
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
       <c r="J39" s="1"/>
       <c r="L39" s="17"/>
     </row>
@@ -1947,10 +1947,10 @@
       <c r="L40" s="17"/>
     </row>
     <row r="41" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G41" s="45" t="s">
+      <c r="G41" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H41" s="46"/>
+      <c r="H41" s="61"/>
       <c r="I41" s="16"/>
       <c r="J41" s="3">
         <f>J31+J33+J36+J37+J34+J35+J38+J39</f>
@@ -1966,18 +1966,6 @@
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="27">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B28:E28"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="B36:E36"/>
@@ -1993,6 +1981,18 @@
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>